<commit_message>
fixed issue with straight party tickets
</commit_message>
<xml_diff>
--- a/MI_Ingham/MI_Ingham_GE20_cleaned.xlsx
+++ b/MI_Ingham/MI_Ingham_GE20_cleaned.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GITREPOS\gh_kessler\openelections_work\MI_Ingham\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02F175B1-0264-422D-8822-5EE17F13E341}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B4D6CD5-A215-480E-9485-2706D655D1EA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2230" yWindow="310" windowWidth="33950" windowHeight="18620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2230" yWindow="310" windowWidth="33950" windowHeight="18620" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="total_reg_and_cast" sheetId="2" r:id="rId1"/>
     <sheet name="straightparty" sheetId="3" r:id="rId2"/>
     <sheet name="presidential" sheetId="4" r:id="rId3"/>
-    <sheet name="usssenate" sheetId="5" r:id="rId4"/>
+    <sheet name="ussenate" sheetId="5" r:id="rId4"/>
     <sheet name="cd08" sheetId="6" r:id="rId5"/>
     <sheet name="statehou67" sheetId="7" r:id="rId6"/>
     <sheet name="statehou68" sheetId="8" r:id="rId7"/>
@@ -30,9 +30,19 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">statehou69!$A$1:$D$153</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">straightparty!$A$1:$B$461</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">total_reg_and_cast!$A$1:$C$461</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">usssenate!$A$1:$F$461</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">ussenate!$A$1:$F$461</definedName>
   </definedNames>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -945,7 +955,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB36813B-EC60-422E-A150-083C026C69FF}">
   <dimension ref="A1:C461"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
@@ -24539,7 +24549,7 @@
   <dimension ref="A1:F461"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.3"/>
@@ -39009,8 +39019,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60CD0B3F-C266-4932-88ED-A168D39CD16C}">
   <dimension ref="A1:C157"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.3"/>

</xml_diff>